<commit_message>
Scénáře a Use Case
</commit_message>
<xml_diff>
--- a/Výkazy/Honza Vrátník.xlsx
+++ b/Výkazy/Honza Vrátník.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Výkaz:</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>Aktualizace naší dokumentace 2. iterace, oprava BDM, BPM, generování dokumentace</t>
+  </si>
+  <si>
+    <t>Oprava 2. iterace - Analytický, BDM, BPM</t>
+  </si>
+  <si>
+    <t>Oprava 2. iterace - Úprava scénářů a Use Case</t>
   </si>
 </sst>
 </file>
@@ -467,7 +473,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,7 +501,7 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <f>SUM(B7:B1002)</f>
-        <v>29</v>
+        <v>30.5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -638,10 +644,20 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="10"/>
+      <c r="A23" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="10"/>
+      <c r="A24" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="10">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>

</xml_diff>

<commit_message>
Moar Code - rezervace stolů
Kalendář, rezervace (add, delete, show)
</commit_message>
<xml_diff>
--- a/Výkazy/Honza Vrátník.xlsx
+++ b/Výkazy/Honza Vrátník.xlsx
@@ -88,7 +88,7 @@
     <t>JaffaPlus - Částečná implementace rezervací stolů</t>
   </si>
   <si>
-    <t>3. iterace - modely balíků</t>
+    <t>3. iterace - modely balíků, pár dalších scénářů</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,7 +507,7 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <f>SUM(B7:B1002)</f>
-        <v>34.5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -678,7 +678,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="10">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Sekvenční diagramy a jeden scénář
</commit_message>
<xml_diff>
--- a/Výkazy/Honza Vrátník.xlsx
+++ b/Výkazy/Honza Vrátník.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Výkaz:</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>3. iterace -  JaffaPlus - implementace Rezervačního systému (přidat, odebrat, prohlížet)</t>
+  </si>
+  <si>
+    <t>3. iterace - sekvenční diagramy a jeden scénář</t>
   </si>
 </sst>
 </file>
@@ -482,7 +485,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,7 +513,7 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <f>SUM(B7:B1002)</f>
-        <v>39</v>
+        <v>40.5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -693,7 +696,12 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="10"/>
+      <c r="A28" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="10">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" s="10"/>

</xml_diff>

<commit_message>
Model návrhových tříd, Zpráva o implementaci
</commit_message>
<xml_diff>
--- a/Výkazy/Honza Vrátník.xlsx
+++ b/Výkazy/Honza Vrátník.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Výkaz:</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t>3. iterace - sekvenční diagramy a jeden scénář</t>
+  </si>
+  <si>
+    <t>3. iterace - diagramy komponent</t>
+  </si>
+  <si>
+    <t>3. iterace - návrhové třídy</t>
   </si>
 </sst>
 </file>
@@ -485,7 +491,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
+      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,7 +519,7 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <f>SUM(B7:B1002)</f>
-        <v>40.5</v>
+        <v>42.5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -704,10 +710,20 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="10"/>
+      <c r="A29" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="10"/>
+      <c r="A30" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31" s="10"/>

</xml_diff>

<commit_message>
Editace rezervace, seřazení rezervací podle času
</commit_message>
<xml_diff>
--- a/Výkazy/Honza Vrátník.xlsx
+++ b/Výkazy/Honza Vrátník.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Výkaz:</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>3. iterace - návrhové třídy</t>
+  </si>
+  <si>
+    <t>4. iterace - další implementace (vybrat stůl)</t>
   </si>
 </sst>
 </file>
@@ -491,7 +494,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,7 +522,7 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <f>SUM(B7:B1002)</f>
-        <v>42.5</v>
+        <v>43.5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -726,7 +729,12 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="10"/>
+      <c r="A31" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B32" s="10"/>

</xml_diff>

<commit_message>
Code Cleanup, Příprava editoru jídelního lístku
</commit_message>
<xml_diff>
--- a/Výkazy/Honza Vrátník.xlsx
+++ b/Výkazy/Honza Vrátník.xlsx
@@ -103,7 +103,7 @@
     <t>3. iterace - návrhové třídy</t>
   </si>
   <si>
-    <t>4. iterace - další implementace (vybrat stůl)</t>
+    <t>4. iterace - další implementace (vybrat stůl, upravit rezervaci)</t>
   </si>
 </sst>
 </file>
@@ -494,7 +494,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,7 +522,7 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <f>SUM(B7:B1002)</f>
-        <v>43.5</v>
+        <v>44.5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -733,10 +733,11 @@
         <v>29</v>
       </c>
       <c r="B31" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
       <c r="B32" s="10"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>